<commit_message>
build: update test database with dummy step
</commit_message>
<xml_diff>
--- a/apps/probable-system/assets/data_files/db.xlsx
+++ b/apps/probable-system/assets/data_files/db.xlsx
@@ -11,15 +11,41 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+  <si>
+    <t>random-id</t>
+  </si>
+  <si>
+    <t>random-test-id</t>
+  </si>
+  <si>
+    <t>test-action</t>
+  </si>
+  <si>
+    <t>random description</t>
+  </si>
+  <si>
+    <t>random_runner_name</t>
+  </si>
+  <si>
+    <t>PENDING</t>
+  </si>
+  <si>
+    <t>random data</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <color theme="1"/>
       <name val="Arial"/>
     </font>
   </fonts>
@@ -37,9 +63,12 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -256,7 +285,31 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
refactor: create test case table in data file
</commit_message>
<xml_diff>
--- a/apps/probable-system/assets/data_files/db.xlsx
+++ b/apps/probable-system/assets/data_files/db.xlsx
@@ -4,6 +4,7 @@
   <workbookPr/>
   <sheets>
     <sheet state="visible" name="test_step_table" sheetId="1" r:id="rId4"/>
+    <sheet state="visible" name="test_case_table" sheetId="2" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -11,9 +12,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
-  <si>
-    <t>random-id</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="18">
+  <si>
+    <t>random-step-id</t>
   </si>
   <si>
     <t>random-test-id</t>
@@ -32,18 +33,52 @@
   </si>
   <si>
     <t>random data</t>
+  </si>
+  <si>
+    <t>random-step-2-id</t>
+  </si>
+  <si>
+    <t>test-action-2</t>
+  </si>
+  <si>
+    <t>random description 2</t>
+  </si>
+  <si>
+    <t>random_runner_2_name</t>
+  </si>
+  <si>
+    <t>random data 2</t>
+  </si>
+  <si>
+    <t>random-step-3-id</t>
+  </si>
+  <si>
+    <t>random description 3</t>
+  </si>
+  <si>
+    <t>random_runner_3_name</t>
+  </si>
+  <si>
+    <t>random data 3</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>random-step-id,random-step-2-id,random-step-3-id</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
+    <font/>
     <font>
       <color theme="1"/>
       <name val="Arial"/>
@@ -63,11 +98,14 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -79,6 +117,10 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -309,6 +351,84 @@
         <v>6</v>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="4" max="4" width="44.0"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
fix(probable_system/assets/data_file): account for data model updates
Update data base to account for changes in the data models for
"test action entity", "test case entity", "test step entity".

Refs e6ce648
Refs 8e74818
Refs bfa8809
</commit_message>
<xml_diff>
--- a/apps/probable-system/assets/data_files/db.xlsx
+++ b/apps/probable-system/assets/data_files/db.xlsx
@@ -4,7 +4,8 @@
   <workbookPr/>
   <sheets>
     <sheet state="visible" name="test_step_table" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="test_case_table" sheetId="2" r:id="rId5"/>
+    <sheet state="visible" name="test_action_table" sheetId="2" r:id="rId5"/>
+    <sheet state="visible" name="test_case_table" sheetId="3" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -12,60 +13,75 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="18">
-  <si>
-    <t>random-step-id</t>
-  </si>
-  <si>
-    <t>random-test-id</t>
-  </si>
-  <si>
-    <t>test-action</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="23">
+  <si>
+    <t>random-step-1-id</t>
+  </si>
+  <si>
+    <t>random-test-id-1</t>
+  </si>
+  <si>
+    <t>random-action-id-1</t>
   </si>
   <si>
     <t>random description</t>
   </si>
   <si>
-    <t>random_runner_name</t>
-  </si>
-  <si>
-    <t>PENDING</t>
-  </si>
-  <si>
-    <t>random data</t>
+    <t>random data 1</t>
   </si>
   <si>
     <t>random-step-2-id</t>
   </si>
   <si>
-    <t>test-action-2</t>
+    <t>random-action-id-2</t>
   </si>
   <si>
     <t>random description 2</t>
   </si>
   <si>
-    <t>random_runner_2_name</t>
-  </si>
-  <si>
     <t>random data 2</t>
   </si>
   <si>
     <t>random-step-3-id</t>
   </si>
   <si>
+    <t>random-action-id-3</t>
+  </si>
+  <si>
     <t>random description 3</t>
   </si>
   <si>
-    <t>random_runner_3_name</t>
-  </si>
-  <si>
     <t>random data 3</t>
   </si>
   <si>
+    <t>random action 1 name</t>
+  </si>
+  <si>
+    <t>random action description 1</t>
+  </si>
+  <si>
+    <t>random_action_runner_1_name</t>
+  </si>
+  <si>
+    <t>random action 2 name</t>
+  </si>
+  <si>
+    <t>random action description 2</t>
+  </si>
+  <si>
+    <t>random_action_runner_2_name</t>
+  </si>
+  <si>
+    <t>random action 3 name</t>
+  </si>
+  <si>
+    <t>random action description 3</t>
+  </si>
+  <si>
+    <t>random_action_runner_3_name</t>
+  </si>
+  <si>
     <t>description</t>
-  </si>
-  <si>
-    <t>random-step-id,random-step-2-id,random-step-3-id</t>
   </si>
 </sst>
 </file>
@@ -121,6 +137,10 @@
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -327,6 +347,11 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="15.57"/>
+    <col customWidth="1" min="3" max="3" width="17.14"/>
+    <col customWidth="1" min="4" max="4" width="18.86"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
@@ -338,63 +363,45 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="B2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="1" t="s">
+      <c r="D2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="E2" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H2" s="1" t="s">
+      <c r="D3" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="1" t="s">
+      <c r="E3" s="2" t="s">
         <v>12</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -412,21 +419,75 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="4" max="4" width="44.0"/>
+    <col customWidth="1" min="1" max="1" width="17.14"/>
+    <col customWidth="1" min="2" max="2" width="18.57"/>
+    <col customWidth="1" min="3" max="3" width="24.57"/>
+    <col customWidth="1" min="4" max="4" width="28.29"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>